<commit_message>
remove 4 columns from all CPs (vol min vol max laterality and number of parts)
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/check_protocol/ORL.xlsx
+++ b/Plancheck/plancheck_data/check_protocol/ORL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="193">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -92,24 +92,6 @@
   </si>
   <si>
     <t>zzExt_ORFIT</t>
-  </si>
-  <si>
-    <t>vol min</t>
-  </si>
-  <si>
-    <t>vol max</t>
-  </si>
-  <si>
-    <t>Expected part</t>
-  </si>
-  <si>
-    <t>Left/right</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>L</t>
   </si>
   <si>
     <t>Contrainte 1</t>
@@ -1629,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
@@ -1734,10 +1716,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
@@ -1748,10 +1730,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -1765,10 +1747,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -1807,7 +1789,7 @@
       <c r="G13" s="32"/>
       <c r="H13" s="33"/>
       <c r="L13" s="16" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1819,7 +1801,7 @@
       <c r="G14" s="32"/>
       <c r="H14" s="33"/>
       <c r="L14" s="16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1831,12 +1813,12 @@
       <c r="G15" s="32"/>
       <c r="H15" s="33"/>
       <c r="L15" s="16" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
@@ -1846,15 +1828,15 @@
       <c r="G16" s="32"/>
       <c r="H16" s="33"/>
       <c r="L16" s="16" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="30"/>
@@ -1863,15 +1845,15 @@
       <c r="G17" s="30"/>
       <c r="H17" s="31"/>
       <c r="L17" s="16" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="30"/>
@@ -1880,15 +1862,15 @@
       <c r="G18" s="30"/>
       <c r="H18" s="31"/>
       <c r="L18" s="16" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="30"/>
@@ -1897,15 +1879,15 @@
       <c r="G19" s="30"/>
       <c r="H19" s="31"/>
       <c r="L19" s="16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="30"/>
@@ -1916,10 +1898,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C21" s="31"/>
       <c r="D21" s="30"/>
@@ -1928,15 +1910,15 @@
       <c r="G21" s="30"/>
       <c r="H21" s="31"/>
       <c r="L21" s="16" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C22" s="31"/>
       <c r="D22" s="30"/>
@@ -1945,15 +1927,15 @@
       <c r="G22" s="30"/>
       <c r="H22" s="31"/>
       <c r="L22" s="16" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="30"/>
@@ -1962,15 +1944,15 @@
       <c r="G23" s="30"/>
       <c r="H23" s="31"/>
       <c r="L23" s="16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="30"/>
@@ -1981,10 +1963,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C25" s="31"/>
       <c r="D25" s="30"/>
@@ -1995,7 +1977,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B26" s="30">
         <v>200</v>
@@ -2007,12 +1989,12 @@
       <c r="G26" s="30"/>
       <c r="H26" s="31"/>
       <c r="L26" s="16" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B27" s="30">
         <v>200</v>
@@ -2024,15 +2006,15 @@
       <c r="G27" s="30"/>
       <c r="H27" s="31"/>
       <c r="L27" s="16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
@@ -2041,7 +2023,7 @@
       <c r="G28" s="30"/>
       <c r="H28" s="30"/>
       <c r="L28" s="16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2053,12 +2035,12 @@
       <c r="G29" s="32"/>
       <c r="H29" s="32"/>
       <c r="L29" s="16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -2068,7 +2050,7 @@
       <c r="G30" s="32"/>
       <c r="H30" s="32"/>
       <c r="L30" s="16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2085,12 +2067,12 @@
       <c r="G31" s="27"/>
       <c r="H31" s="27"/>
       <c r="L31" s="16" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B32" s="27">
         <v>0.125</v>
@@ -2102,12 +2084,12 @@
       <c r="G32" s="27"/>
       <c r="H32" s="27"/>
       <c r="L32" s="16" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B33" s="27">
         <v>0.125</v>
@@ -2119,12 +2101,12 @@
       <c r="G33" s="27"/>
       <c r="H33" s="27"/>
       <c r="L33" s="16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>5</v>
@@ -2136,12 +2118,12 @@
       <c r="G34" s="27"/>
       <c r="H34" s="27"/>
       <c r="L34" s="16" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>6</v>
@@ -2153,7 +2135,7 @@
       <c r="G35" s="27"/>
       <c r="H35" s="27"/>
       <c r="L35" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2166,7 +2148,7 @@
       <c r="G36" s="27"/>
       <c r="H36" s="27"/>
       <c r="L36" s="16" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2179,7 +2161,7 @@
       <c r="G37" s="27"/>
       <c r="H37" s="27"/>
       <c r="L37" s="16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2192,7 +2174,7 @@
       <c r="G38" s="27"/>
       <c r="H38" s="27"/>
       <c r="L38" s="16" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2205,7 +2187,7 @@
       <c r="G39" s="27"/>
       <c r="H39" s="27"/>
       <c r="L39" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2218,7 +2200,7 @@
       <c r="G40" s="27"/>
       <c r="H40" s="27"/>
       <c r="L40" s="16" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2231,20 +2213,20 @@
       <c r="G41" s="27"/>
       <c r="H41" s="27"/>
       <c r="L41" s="16" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C44" s="24"/>
       <c r="D44" s="24"/>
@@ -2255,7 +2237,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B45" s="23">
         <v>300</v>
@@ -2269,7 +2251,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B46" s="23">
         <v>3</v>
@@ -2283,7 +2265,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B47" s="23">
         <v>100</v>
@@ -2297,7 +2279,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B48" s="23">
         <v>30</v>
@@ -2309,12 +2291,12 @@
       <c r="G48" s="24"/>
       <c r="H48" s="24"/>
       <c r="L48" s="16" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B49" s="23">
         <v>0.1</v>
@@ -2326,52 +2308,52 @@
       <c r="G49" s="24"/>
       <c r="H49" s="24"/>
       <c r="L49" s="16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L51" s="16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L52" s="16" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L55" s="16" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L56" s="16" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L57" s="16" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L58" s="16" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L59" s="16" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L60" s="16" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L61" s="16" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2411,21 +2393,19 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="11" customWidth="1"/>
-    <col min="2" max="4" width="11.42578125" style="12"/>
-    <col min="5" max="5" width="15.42578125" style="12" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="12"/>
+    <col min="2" max="16384" width="11.42578125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
@@ -2433,330 +2413,192 @@
         <v>20</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E2" s="12">
-        <v>1</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="12">
-        <v>1</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E4" s="12">
-        <v>1</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E5" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="12">
-        <v>1</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="E13" s="12">
-        <v>1</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="12">
-        <v>1</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="E15" s="12">
-        <v>1</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
         <f>"Oesophage"</f>
         <v>Oesophage</v>
       </c>
-      <c r="E16" s="12">
-        <v>1</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E17" s="12">
-        <v>1</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="12">
-        <v>1</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E19" s="12">
-        <v>1</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="E20" s="12">
-        <v>1</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="E21" s="12">
-        <v>1</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="E22" s="12">
-        <v>1</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="E23" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="E24" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="E25" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="E26" s="12">
-        <v>1</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
         <v>174</v>
-      </c>
-      <c r="E27" s="12">
-        <v>1</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="E28" s="12">
-        <v>1</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="E29" s="12">
-        <v>1</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="E30" s="12">
-        <v>1</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="E31" s="12">
-        <v>1</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="E32" s="12">
-        <v>1</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="E33" s="12">
-        <v>1</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2770,19 +2612,18 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -2790,229 +2631,175 @@
         <v>20</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="F17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="F18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -3025,19 +2812,18 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -3045,63 +2831,51 @@
         <v>20</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B2">
         <v>-1000</v>
       </c>
-      <c r="G2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B3">
         <v>-300</v>
       </c>
-      <c r="G3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B5">
         <v>-900</v>
       </c>
-      <c r="G5" t="s">
-        <v>96</v>
+      <c r="C5" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -3116,7 +2890,7 @@
   </sheetPr>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -3133,128 +2907,128 @@
         <v>2</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C8" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12"/>
@@ -3263,59 +3037,59 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -3324,72 +3098,72 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C25" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>